<commit_message>
dev changes + new db files
</commit_message>
<xml_diff>
--- a/Curves_Budget_Response.xlsx
+++ b/Curves_Budget_Response.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I658"/>
+  <dimension ref="A1:I725"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -23470,6 +23470,2351 @@
         </is>
       </c>
     </row>
+    <row r="659">
+      <c r="A659" s="1" t="n">
+        <v>657</v>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>region: France24 brand: Lion budget: 100000</t>
+        </is>
+      </c>
+      <c r="C659" t="n">
+        <v>100000.0000010221</v>
+      </c>
+      <c r="D659" t="n">
+        <v>125250.1466502521</v>
+      </c>
+      <c r="E659" t="n">
+        <v>195294.937532378</v>
+      </c>
+      <c r="F659" t="n">
+        <v>320545.0841826301</v>
+      </c>
+      <c r="G659" t="n">
+        <v>600774.7688511446</v>
+      </c>
+      <c r="H659" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I659" t="inlineStr">
+        <is>
+          <t>Lion</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" s="1" t="n">
+        <v>658</v>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>region: France24 brand: Lion budget: 200000</t>
+        </is>
+      </c>
+      <c r="C660" t="n">
+        <v>200000.0000000123</v>
+      </c>
+      <c r="D660" t="n">
+        <v>209034.7695164511</v>
+      </c>
+      <c r="E660" t="n">
+        <v>312994.2553459719</v>
+      </c>
+      <c r="F660" t="n">
+        <v>522029.0248624231</v>
+      </c>
+      <c r="G660" t="n">
+        <v>774522.6180037796</v>
+      </c>
+      <c r="H660" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I660" t="inlineStr">
+        <is>
+          <t>Lion</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" s="1" t="n">
+        <v>659</v>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>region: France24 brand: Lion budget: 300000</t>
+        </is>
+      </c>
+      <c r="C661" t="n">
+        <v>300000.0000000095</v>
+      </c>
+      <c r="D661" t="n">
+        <v>271382.8723251</v>
+      </c>
+      <c r="E661" t="n">
+        <v>403686.0921449232</v>
+      </c>
+      <c r="F661" t="n">
+        <v>675068.9644700232</v>
+      </c>
+      <c r="G661" t="n">
+        <v>824771.5909160736</v>
+      </c>
+      <c r="H661" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I661" t="inlineStr">
+        <is>
+          <t>Lion</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" s="1" t="n">
+        <v>660</v>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>region: France24 brand: Lion budget: 400000</t>
+        </is>
+      </c>
+      <c r="C662" t="n">
+        <v>400000.000000092</v>
+      </c>
+      <c r="D662" t="n">
+        <v>319449.1050270235</v>
+      </c>
+      <c r="E662" t="n">
+        <v>486745.9308518922</v>
+      </c>
+      <c r="F662" t="n">
+        <v>806195.0358789158</v>
+      </c>
+      <c r="G662" t="n">
+        <v>839303.9105448422</v>
+      </c>
+      <c r="H662" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I662" t="inlineStr">
+        <is>
+          <t>Lion</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" s="1" t="n">
+        <v>661</v>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>region: France24 brand: Lion budget: 500000</t>
+        </is>
+      </c>
+      <c r="C663" t="n">
+        <v>500000.0000000459</v>
+      </c>
+      <c r="D663" t="n">
+        <v>365236.6671771041</v>
+      </c>
+      <c r="E663" t="n">
+        <v>558256.0959836208</v>
+      </c>
+      <c r="F663" t="n">
+        <v>923492.7631607249</v>
+      </c>
+      <c r="G663" t="n">
+        <v>843506.7489622734</v>
+      </c>
+      <c r="H663" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I663" t="inlineStr">
+        <is>
+          <t>Lion</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" s="1" t="n">
+        <v>662</v>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>region: France24 brand: Lion budget: 600000</t>
+        </is>
+      </c>
+      <c r="C664" t="n">
+        <v>600000.0000000102</v>
+      </c>
+      <c r="D664" t="n">
+        <v>406964.1286149482</v>
+      </c>
+      <c r="E664" t="n">
+        <v>623314.4375618057</v>
+      </c>
+      <c r="F664" t="n">
+        <v>1030278.566176754</v>
+      </c>
+      <c r="G664" t="n">
+        <v>844722.2363183392</v>
+      </c>
+      <c r="H664" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I664" t="inlineStr">
+        <is>
+          <t>Lion</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" s="1" t="n">
+        <v>663</v>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>region: France24 brand: Lion budget: 700000</t>
+        </is>
+      </c>
+      <c r="C665" t="n">
+        <v>700000.0000001403</v>
+      </c>
+      <c r="D665" t="n">
+        <v>444485.5282120819</v>
+      </c>
+      <c r="E665" t="n">
+        <v>683685.8165004452</v>
+      </c>
+      <c r="F665" t="n">
+        <v>1128171.344712527</v>
+      </c>
+      <c r="G665" t="n">
+        <v>845073.762921558</v>
+      </c>
+      <c r="H665" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I665" t="inlineStr">
+        <is>
+          <t>Lion</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" s="1" t="n">
+        <v>664</v>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>region: France24 brand: Chocapic budget: 100000</t>
+        </is>
+      </c>
+      <c r="C666" t="n">
+        <v>100000</v>
+      </c>
+      <c r="D666" t="n">
+        <v>102094.706309181</v>
+      </c>
+      <c r="E666" t="n">
+        <v>85487.68795893951</v>
+      </c>
+      <c r="F666" t="n">
+        <v>187582.3942681205</v>
+      </c>
+      <c r="G666" t="n">
+        <v>524941.806984932</v>
+      </c>
+      <c r="H666" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I666" t="inlineStr">
+        <is>
+          <t>Chocapic</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" s="1" t="n">
+        <v>665</v>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>region: France24 brand: Chocapic budget: 1000000</t>
+        </is>
+      </c>
+      <c r="C667" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="D667" t="n">
+        <v>759036.0992668523</v>
+      </c>
+      <c r="E667" t="n">
+        <v>420712.6816421038</v>
+      </c>
+      <c r="F667" t="n">
+        <v>1179748.780908956</v>
+      </c>
+      <c r="G667" t="n">
+        <v>2136742.111652715</v>
+      </c>
+      <c r="H667" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I667" t="inlineStr">
+        <is>
+          <t>Chocapic</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" s="1" t="n">
+        <v>666</v>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>region: France24 brand: Chocapic budget: 1100000</t>
+        </is>
+      </c>
+      <c r="C668" t="n">
+        <v>1100000</v>
+      </c>
+      <c r="D668" t="n">
+        <v>822803.8634842605</v>
+      </c>
+      <c r="E668" t="n">
+        <v>457411.8943953955</v>
+      </c>
+      <c r="F668" t="n">
+        <v>1280215.757879656</v>
+      </c>
+      <c r="G668" t="n">
+        <v>2176754.935727349</v>
+      </c>
+      <c r="H668" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I668" t="inlineStr">
+        <is>
+          <t>Chocapic</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" s="1" t="n">
+        <v>667</v>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>region: France24 brand: Chocapic budget: 1200000</t>
+        </is>
+      </c>
+      <c r="C669" t="n">
+        <v>1200000</v>
+      </c>
+      <c r="D669" t="n">
+        <v>884944.7329684747</v>
+      </c>
+      <c r="E669" t="n">
+        <v>494003.549771946</v>
+      </c>
+      <c r="F669" t="n">
+        <v>1378948.282740421</v>
+      </c>
+      <c r="G669" t="n">
+        <v>2207686.936254741</v>
+      </c>
+      <c r="H669" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I669" t="inlineStr">
+        <is>
+          <t>Chocapic</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" s="1" t="n">
+        <v>668</v>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>region: France24 brand: Chocapic budget: 1300000</t>
+        </is>
+      </c>
+      <c r="C670" t="n">
+        <v>1300000.000002096</v>
+      </c>
+      <c r="D670" t="n">
+        <v>945513.3430057914</v>
+      </c>
+      <c r="E670" t="n">
+        <v>530486.3755503903</v>
+      </c>
+      <c r="F670" t="n">
+        <v>1475999.718556182</v>
+      </c>
+      <c r="G670" t="n">
+        <v>2231598.986422944</v>
+      </c>
+      <c r="H670" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I670" t="inlineStr">
+        <is>
+          <t>Chocapic</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" s="1" t="n">
+        <v>669</v>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>region: France24 brand: Chocapic budget: 1400000</t>
+        </is>
+      </c>
+      <c r="C671" t="n">
+        <v>1400000</v>
+      </c>
+      <c r="D671" t="n">
+        <v>1004559.007319402</v>
+      </c>
+      <c r="E671" t="n">
+        <v>566862.4227880922</v>
+      </c>
+      <c r="F671" t="n">
+        <v>1571421.430107494</v>
+      </c>
+      <c r="G671" t="n">
+        <v>2250084.248722927</v>
+      </c>
+      <c r="H671" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I671" t="inlineStr">
+        <is>
+          <t>Chocapic</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" s="1" t="n">
+        <v>670</v>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>region: France24 brand: Chocapic budget: 1500000</t>
+        </is>
+      </c>
+      <c r="C672" t="n">
+        <v>1500000.000001412</v>
+      </c>
+      <c r="D672" t="n">
+        <v>1062131.301902639</v>
+      </c>
+      <c r="E672" t="n">
+        <v>603131.5655991172</v>
+      </c>
+      <c r="F672" t="n">
+        <v>1665262.867501756</v>
+      </c>
+      <c r="G672" t="n">
+        <v>2264374.320879949</v>
+      </c>
+      <c r="H672" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I672" t="inlineStr">
+        <is>
+          <t>Chocapic</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" s="1" t="n">
+        <v>671</v>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>region: France24 brand: Chocapic budget: 1600000</t>
+        </is>
+      </c>
+      <c r="C673" t="n">
+        <v>1600000.000004794</v>
+      </c>
+      <c r="D673" t="n">
+        <v>1118277.504075567</v>
+      </c>
+      <c r="E673" t="n">
+        <v>639294.1413223908</v>
+      </c>
+      <c r="F673" t="n">
+        <v>1757571.645397957</v>
+      </c>
+      <c r="G673" t="n">
+        <v>2275421.292187922</v>
+      </c>
+      <c r="H673" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I673" t="inlineStr">
+        <is>
+          <t>Chocapic</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" s="1" t="n">
+        <v>672</v>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>region: France24 brand: Chocapic budget: 1700000</t>
+        </is>
+      </c>
+      <c r="C674" t="n">
+        <v>1700000</v>
+      </c>
+      <c r="D674" t="n">
+        <v>1173036.933268335</v>
+      </c>
+      <c r="E674" t="n">
+        <v>675356.7129060673</v>
+      </c>
+      <c r="F674" t="n">
+        <v>1848393.646174402</v>
+      </c>
+      <c r="G674" t="n">
+        <v>2283961.177342229</v>
+      </c>
+      <c r="H674" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I674" t="inlineStr">
+        <is>
+          <t>Chocapic</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" s="1" t="n">
+        <v>673</v>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>region: France24 brand: Chocapic budget: 1800000</t>
+        </is>
+      </c>
+      <c r="C675" t="n">
+        <v>1800000.000000017</v>
+      </c>
+      <c r="D675" t="n">
+        <v>1226329.109696778</v>
+      </c>
+      <c r="E675" t="n">
+        <v>711465.2349224939</v>
+      </c>
+      <c r="F675" t="n">
+        <v>1937794.344619272</v>
+      </c>
+      <c r="G675" t="n">
+        <v>2290562.954103063</v>
+      </c>
+      <c r="H675" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I675" t="inlineStr">
+        <is>
+          <t>Chocapic</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" s="1" t="n">
+        <v>674</v>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>region: France24 brand: Chocapic budget: 1900000</t>
+        </is>
+      </c>
+      <c r="C676" t="n">
+        <v>1900000</v>
+      </c>
+      <c r="D676" t="n">
+        <v>1278383.521142295</v>
+      </c>
+      <c r="E676" t="n">
+        <v>747449.4389882454</v>
+      </c>
+      <c r="F676" t="n">
+        <v>2025832.96013054</v>
+      </c>
+      <c r="G676" t="n">
+        <v>2295666.471961909</v>
+      </c>
+      <c r="H676" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I676" t="inlineStr">
+        <is>
+          <t>Chocapic</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" s="1" t="n">
+        <v>675</v>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>region: France24 brand: Chocapic budget: 200000</t>
+        </is>
+      </c>
+      <c r="C677" t="n">
+        <v>200000</v>
+      </c>
+      <c r="D677" t="n">
+        <v>183258.7676778982</v>
+      </c>
+      <c r="E677" t="n">
+        <v>123178.1809425792</v>
+      </c>
+      <c r="F677" t="n">
+        <v>306436.9486204774</v>
+      </c>
+      <c r="G677" t="n">
+        <v>930749.2106368382</v>
+      </c>
+      <c r="H677" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I677" t="inlineStr">
+        <is>
+          <t>Chocapic</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" s="1" t="n">
+        <v>676</v>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>region: France24 brand: Chocapic budget: 2000000</t>
+        </is>
+      </c>
+      <c r="C678" t="n">
+        <v>2000000.000009032</v>
+      </c>
+      <c r="D678" t="n">
+        <v>1329237.156890679</v>
+      </c>
+      <c r="E678" t="n">
+        <v>783310.8353663606</v>
+      </c>
+      <c r="F678" t="n">
+        <v>2112547.992257039</v>
+      </c>
+      <c r="G678" t="n">
+        <v>2299611.757523845</v>
+      </c>
+      <c r="H678" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I678" t="inlineStr">
+        <is>
+          <t>Chocapic</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" s="1" t="n">
+        <v>677</v>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>region: France24 brand: Chocapic budget: 2100000</t>
+        </is>
+      </c>
+      <c r="C679" t="n">
+        <v>2100000.000000014</v>
+      </c>
+      <c r="D679" t="n">
+        <v>1378925.852325627</v>
+      </c>
+      <c r="E679" t="n">
+        <v>819050.7440060833</v>
+      </c>
+      <c r="F679" t="n">
+        <v>2197976.596331711</v>
+      </c>
+      <c r="G679" t="n">
+        <v>2302661.669093014</v>
+      </c>
+      <c r="H679" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I679" t="inlineStr">
+        <is>
+          <t>Chocapic</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" s="1" t="n">
+        <v>678</v>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>region: France24 brand: Chocapic budget: 2200000</t>
+        </is>
+      </c>
+      <c r="C680" t="n">
+        <v>2200000</v>
+      </c>
+      <c r="D680" t="n">
+        <v>1427484.083610175</v>
+      </c>
+      <c r="E680" t="n">
+        <v>854670.552330671</v>
+      </c>
+      <c r="F680" t="n">
+        <v>2282154.635940847</v>
+      </c>
+      <c r="G680" t="n">
+        <v>2305019.409853819</v>
+      </c>
+      <c r="H680" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I680" t="inlineStr">
+        <is>
+          <t>Chocapic</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" s="1" t="n">
+        <v>679</v>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>region: France24 brand: Chocapic budget: 2300000</t>
+        </is>
+      </c>
+      <c r="C681" t="n">
+        <v>2300000.000000071</v>
+      </c>
+      <c r="D681" t="n">
+        <v>1474945.240807915</v>
+      </c>
+      <c r="E681" t="n">
+        <v>890171.4922615559</v>
+      </c>
+      <c r="F681" t="n">
+        <v>2365116.733069471</v>
+      </c>
+      <c r="G681" t="n">
+        <v>2306842.066468125</v>
+      </c>
+      <c r="H681" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I681" t="inlineStr">
+        <is>
+          <t>Chocapic</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" s="1" t="n">
+        <v>680</v>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>region: France24 brand: Chocapic budget: 2400000</t>
+        </is>
+      </c>
+      <c r="C682" t="n">
+        <v>2400000</v>
+      </c>
+      <c r="D682" t="n">
+        <v>1521341.494152786</v>
+      </c>
+      <c r="E682" t="n">
+        <v>925554.8221233945</v>
+      </c>
+      <c r="F682" t="n">
+        <v>2446896.316276181</v>
+      </c>
+      <c r="G682" t="n">
+        <v>2308251.075121195</v>
+      </c>
+      <c r="H682" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I682" t="inlineStr">
+        <is>
+          <t>Chocapic</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" s="1" t="n">
+        <v>681</v>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>region: France24 brand: Chocapic budget: 2500000</t>
+        </is>
+      </c>
+      <c r="C683" t="n">
+        <v>2500000.000000064</v>
+      </c>
+      <c r="D683" t="n">
+        <v>1566703.926289873</v>
+      </c>
+      <c r="E683" t="n">
+        <v>960821.7404156253</v>
+      </c>
+      <c r="F683" t="n">
+        <v>2527525.666705498</v>
+      </c>
+      <c r="G683" t="n">
+        <v>2309340.312319714</v>
+      </c>
+      <c r="H683" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I683" t="inlineStr">
+        <is>
+          <t>Chocapic</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" s="1" t="n">
+        <v>682</v>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>region: France24 brand: Chocapic budget: 2600000</t>
+        </is>
+      </c>
+      <c r="C684" t="n">
+        <v>2600000</v>
+      </c>
+      <c r="D684" t="n">
+        <v>1611062.545468493</v>
+      </c>
+      <c r="E684" t="n">
+        <v>995973.4168874458</v>
+      </c>
+      <c r="F684" t="n">
+        <v>2607035.962355939</v>
+      </c>
+      <c r="G684" t="n">
+        <v>2310182.349500998</v>
+      </c>
+      <c r="H684" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I684" t="inlineStr">
+        <is>
+          <t>Chocapic</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" s="1" t="n">
+        <v>683</v>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>region: France24 brand: Chocapic budget: 2700000</t>
+        </is>
+      </c>
+      <c r="C685" t="n">
+        <v>2700000.000000048</v>
+      </c>
+      <c r="D685" t="n">
+        <v>1654446.373518526</v>
+      </c>
+      <c r="E685" t="n">
+        <v>1031010.946789557</v>
+      </c>
+      <c r="F685" t="n">
+        <v>2685457.320308083</v>
+      </c>
+      <c r="G685" t="n">
+        <v>2310833.288172235</v>
+      </c>
+      <c r="H685" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I685" t="inlineStr">
+        <is>
+          <t>Chocapic</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" s="1" t="n">
+        <v>684</v>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>region: France24 brand: Chocapic budget: 2800000</t>
+        </is>
+      </c>
+      <c r="C686" t="n">
+        <v>2800000.000000002</v>
+      </c>
+      <c r="D686" t="n">
+        <v>1696883.411054058</v>
+      </c>
+      <c r="E686" t="n">
+        <v>1065935.426319341</v>
+      </c>
+      <c r="F686" t="n">
+        <v>2762818.837373399</v>
+      </c>
+      <c r="G686" t="n">
+        <v>2311336.497725363</v>
+      </c>
+      <c r="H686" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I686" t="inlineStr">
+        <is>
+          <t>Chocapic</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" s="1" t="n">
+        <v>685</v>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>region: France24 brand: Chocapic budget: 2900000</t>
+        </is>
+      </c>
+      <c r="C687" t="n">
+        <v>2900000.000005581</v>
+      </c>
+      <c r="D687" t="n">
+        <v>1738400.731935557</v>
+      </c>
+      <c r="E687" t="n">
+        <v>1100747.896995901</v>
+      </c>
+      <c r="F687" t="n">
+        <v>2839148.628931458</v>
+      </c>
+      <c r="G687" t="n">
+        <v>2311725.504963005</v>
+      </c>
+      <c r="H687" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I687" t="inlineStr">
+        <is>
+          <t>Chocapic</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" s="1" t="n">
+        <v>686</v>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>region: France24 brand: Chocapic budget: 300000</t>
+        </is>
+      </c>
+      <c r="C688" t="n">
+        <v>300000</v>
+      </c>
+      <c r="D688" t="n">
+        <v>262214.3439261721</v>
+      </c>
+      <c r="E688" t="n">
+        <v>160756.7234639353</v>
+      </c>
+      <c r="F688" t="n">
+        <v>422971.0673901074</v>
+      </c>
+      <c r="G688" t="n">
+        <v>1244459.50512559</v>
+      </c>
+      <c r="H688" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I688" t="inlineStr">
+        <is>
+          <t>Chocapic</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" s="1" t="n">
+        <v>687</v>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>region: France24 brand: Chocapic budget: 3000000</t>
+        </is>
+      </c>
+      <c r="C689" t="n">
+        <v>3000000.000000001</v>
+      </c>
+      <c r="D689" t="n">
+        <v>1779024.510062495</v>
+      </c>
+      <c r="E689" t="n">
+        <v>1135449.356131919</v>
+      </c>
+      <c r="F689" t="n">
+        <v>2914473.866194414</v>
+      </c>
+      <c r="G689" t="n">
+        <v>2312026.227852649</v>
+      </c>
+      <c r="H689" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I689" t="inlineStr">
+        <is>
+          <t>Chocapic</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" s="1" t="n">
+        <v>688</v>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>region: France24 brand: Chocapic budget: 3100000</t>
+        </is>
+      </c>
+      <c r="C690" t="n">
+        <v>3100000.000000002</v>
+      </c>
+      <c r="D690" t="n">
+        <v>1818779.975926069</v>
+      </c>
+      <c r="E690" t="n">
+        <v>1170040.836090124</v>
+      </c>
+      <c r="F690" t="n">
+        <v>2988820.812016193</v>
+      </c>
+      <c r="G690" t="n">
+        <v>2312258.702335437</v>
+      </c>
+      <c r="H690" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I690" t="inlineStr">
+        <is>
+          <t>Chocapic</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" s="1" t="n">
+        <v>689</v>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>region: France24 brand: Chocapic budget: 3200000</t>
+        </is>
+      </c>
+      <c r="C691" t="n">
+        <v>3200000.0000003</v>
+      </c>
+      <c r="D691" t="n">
+        <v>1857691.652548711</v>
+      </c>
+      <c r="E691" t="n">
+        <v>1204523.202557247</v>
+      </c>
+      <c r="F691" t="n">
+        <v>3062214.855105957</v>
+      </c>
+      <c r="G691" t="n">
+        <v>2312438.41723911</v>
+      </c>
+      <c r="H691" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I691" t="inlineStr">
+        <is>
+          <t>Chocapic</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" s="1" t="n">
+        <v>690</v>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>region: France24 brand: Chocapic budget: 3300000</t>
+        </is>
+      </c>
+      <c r="C692" t="n">
+        <v>3300000.000007519</v>
+      </c>
+      <c r="D692" t="n">
+        <v>1895783.143746197</v>
+      </c>
+      <c r="E692" t="n">
+        <v>1238897.399152468</v>
+      </c>
+      <c r="F692" t="n">
+        <v>3134680.542898666</v>
+      </c>
+      <c r="G692" t="n">
+        <v>2312577.346235602</v>
+      </c>
+      <c r="H692" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I692" t="inlineStr">
+        <is>
+          <t>Chocapic</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" s="1" t="n">
+        <v>691</v>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>region: France24 brand: Chocapic budget: 3400000</t>
+        </is>
+      </c>
+      <c r="C693" t="n">
+        <v>3400000.000003136</v>
+      </c>
+      <c r="D693" t="n">
+        <v>1933077.151643984</v>
+      </c>
+      <c r="E693" t="n">
+        <v>1273164.461454954</v>
+      </c>
+      <c r="F693" t="n">
+        <v>3206241.613098938</v>
+      </c>
+      <c r="G693" t="n">
+        <v>2312684.745597972</v>
+      </c>
+      <c r="H693" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I693" t="inlineStr">
+        <is>
+          <t>Chocapic</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" s="1" t="n">
+        <v>692</v>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>region: France24 brand: Chocapic budget: 3500000</t>
+        </is>
+      </c>
+      <c r="C694" t="n">
+        <v>3500000.000000002</v>
+      </c>
+      <c r="D694" t="n">
+        <v>1969595.860620855</v>
+      </c>
+      <c r="E694" t="n">
+        <v>1307325.163290943</v>
+      </c>
+      <c r="F694" t="n">
+        <v>3276921.023911798</v>
+      </c>
+      <c r="G694" t="n">
+        <v>2312767.770908242</v>
+      </c>
+      <c r="H694" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I694" t="inlineStr">
+        <is>
+          <t>Chocapic</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" s="1" t="n">
+        <v>693</v>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>region: France24 brand: Chocapic budget: 3600000</t>
+        </is>
+      </c>
+      <c r="C695" t="n">
+        <v>3600000.000000001</v>
+      </c>
+      <c r="D695" t="n">
+        <v>2005360.847512547</v>
+      </c>
+      <c r="E695" t="n">
+        <v>1341380.135549214</v>
+      </c>
+      <c r="F695" t="n">
+        <v>3346740.983061762</v>
+      </c>
+      <c r="G695" t="n">
+        <v>2312831.953804614</v>
+      </c>
+      <c r="H695" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I695" t="inlineStr">
+        <is>
+          <t>Chocapic</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" s="1" t="n">
+        <v>694</v>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>region: France24 brand: Chocapic budget: 3700000</t>
+        </is>
+      </c>
+      <c r="C696" t="n">
+        <v>3700000.000000004</v>
+      </c>
+      <c r="D696" t="n">
+        <v>2040392.357520424</v>
+      </c>
+      <c r="E696" t="n">
+        <v>1375330.618070021</v>
+      </c>
+      <c r="F696" t="n">
+        <v>3415722.975590444</v>
+      </c>
+      <c r="G696" t="n">
+        <v>2312881.570532009</v>
+      </c>
+      <c r="H696" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I696" t="inlineStr">
+        <is>
+          <t>Chocapic</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" s="1" t="n">
+        <v>695</v>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>region: France24 brand: Chocapic budget: 3800000</t>
+        </is>
+      </c>
+      <c r="C697" t="n">
+        <v>3800000.000001657</v>
+      </c>
+      <c r="D697" t="n">
+        <v>2074710.97211537</v>
+      </c>
+      <c r="E697" t="n">
+        <v>1409176.818502167</v>
+      </c>
+      <c r="F697" t="n">
+        <v>3483887.790617536</v>
+      </c>
+      <c r="G697" t="n">
+        <v>2312919.926850851</v>
+      </c>
+      <c r="H697" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I697" t="inlineStr">
+        <is>
+          <t>Chocapic</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" s="1" t="n">
+        <v>696</v>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>region: France24 brand: Chocapic budget: 3900000</t>
+        </is>
+      </c>
+      <c r="C698" t="n">
+        <v>3900000.000000001</v>
+      </c>
+      <c r="D698" t="n">
+        <v>2108335.571401416</v>
+      </c>
+      <c r="E698" t="n">
+        <v>1442919.975501976</v>
+      </c>
+      <c r="F698" t="n">
+        <v>3551255.546903393</v>
+      </c>
+      <c r="G698" t="n">
+        <v>2312949.578286411</v>
+      </c>
+      <c r="H698" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I698" t="inlineStr">
+        <is>
+          <t>Chocapic</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" s="1" t="n">
+        <v>697</v>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>region: France24 brand: Chocapic budget: 400000</t>
+        </is>
+      </c>
+      <c r="C699" t="n">
+        <v>400000.0000001807</v>
+      </c>
+      <c r="D699" t="n">
+        <v>339036.2151122032</v>
+      </c>
+      <c r="E699" t="n">
+        <v>198224.3331542342</v>
+      </c>
+      <c r="F699" t="n">
+        <v>537260.5482664374</v>
+      </c>
+      <c r="G699" t="n">
+        <v>1486973.929413407</v>
+      </c>
+      <c r="H699" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I699" t="inlineStr">
+        <is>
+          <t>Chocapic</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" s="1" t="n">
+        <v>698</v>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>region: France24 brand: Chocapic budget: 500000</t>
+        </is>
+      </c>
+      <c r="C700" t="n">
+        <v>500000.0000000001</v>
+      </c>
+      <c r="D700" t="n">
+        <v>413797.4571393967</v>
+      </c>
+      <c r="E700" t="n">
+        <v>235580.7845474812</v>
+      </c>
+      <c r="F700" t="n">
+        <v>649378.2416868778</v>
+      </c>
+      <c r="G700" t="n">
+        <v>1674450.231659692</v>
+      </c>
+      <c r="H700" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I700" t="inlineStr">
+        <is>
+          <t>Chocapic</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" s="1" t="n">
+        <v>699</v>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>region: France24 brand: Chocapic budget: 600000</t>
+        </is>
+      </c>
+      <c r="C701" t="n">
+        <v>600000.0000000001</v>
+      </c>
+      <c r="D701" t="n">
+        <v>486567.5899095092</v>
+      </c>
+      <c r="E701" t="n">
+        <v>272826.5871994148</v>
+      </c>
+      <c r="F701" t="n">
+        <v>759394.177108924</v>
+      </c>
+      <c r="G701" t="n">
+        <v>1819379.194163081</v>
+      </c>
+      <c r="H701" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I701" t="inlineStr">
+        <is>
+          <t>Chocapic</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" s="1" t="n">
+        <v>700</v>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>region: France24 brand: Chocapic budget: 700000</t>
+        </is>
+      </c>
+      <c r="C702" t="n">
+        <v>700000.0000000001</v>
+      </c>
+      <c r="D702" t="n">
+        <v>557413.3813803876</v>
+      </c>
+      <c r="E702" t="n">
+        <v>309962.3019368438</v>
+      </c>
+      <c r="F702" t="n">
+        <v>867375.6833172314</v>
+      </c>
+      <c r="G702" t="n">
+        <v>1931416.843298451</v>
+      </c>
+      <c r="H702" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I702" t="inlineStr">
+        <is>
+          <t>Chocapic</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" s="1" t="n">
+        <v>701</v>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>region: France24 brand: Chocapic budget: 800000</t>
+        </is>
+      </c>
+      <c r="C703" t="n">
+        <v>800000.0000000001</v>
+      </c>
+      <c r="D703" t="n">
+        <v>626399.4725840504</v>
+      </c>
+      <c r="E703" t="n">
+        <v>346988.0307325568</v>
+      </c>
+      <c r="F703" t="n">
+        <v>973387.5033166071</v>
+      </c>
+      <c r="G703" t="n">
+        <v>2018027.791220518</v>
+      </c>
+      <c r="H703" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I703" t="inlineStr">
+        <is>
+          <t>Chocapic</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" s="1" t="n">
+        <v>702</v>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>region: France24 brand: Chocapic budget: 900000</t>
+        </is>
+      </c>
+      <c r="C704" t="n">
+        <v>900000.0000035308</v>
+      </c>
+      <c r="D704" t="n">
+        <v>693586.9626307425</v>
+      </c>
+      <c r="E704" t="n">
+        <v>383904.9413614271</v>
+      </c>
+      <c r="F704" t="n">
+        <v>1077491.90399217</v>
+      </c>
+      <c r="G704" t="n">
+        <v>2084982.572564845</v>
+      </c>
+      <c r="H704" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I704" t="inlineStr">
+        <is>
+          <t>Chocapic</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" s="1" t="n">
+        <v>703</v>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>region: France24 brand: KitKat budget: 100000</t>
+        </is>
+      </c>
+      <c r="C705" t="n">
+        <v>100000.0000002172</v>
+      </c>
+      <c r="D705" t="n">
+        <v>0</v>
+      </c>
+      <c r="E705" t="n">
+        <v>53797.14198748449</v>
+      </c>
+      <c r="F705" t="n">
+        <v>53797.14198748449</v>
+      </c>
+      <c r="G705" t="n">
+        <v>98649.39954341293</v>
+      </c>
+      <c r="H705" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I705" t="inlineStr">
+        <is>
+          <t>KitKat</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" s="1" t="n">
+        <v>704</v>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>region: France24 brand: KitKat budget: 1000000</t>
+        </is>
+      </c>
+      <c r="C706" t="n">
+        <v>1000000.000008665</v>
+      </c>
+      <c r="D706" t="n">
+        <v>0</v>
+      </c>
+      <c r="E706" t="n">
+        <v>243279.7768626516</v>
+      </c>
+      <c r="F706" t="n">
+        <v>243279.7768626516</v>
+      </c>
+      <c r="G706" t="n">
+        <v>269377.0024791136</v>
+      </c>
+      <c r="H706" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I706" t="inlineStr">
+        <is>
+          <t>KitKat</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" s="1" t="n">
+        <v>705</v>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>region: France24 brand: KitKat budget: 1100000</t>
+        </is>
+      </c>
+      <c r="C707" t="n">
+        <v>1100000.000004061</v>
+      </c>
+      <c r="D707" t="n">
+        <v>0</v>
+      </c>
+      <c r="E707" t="n">
+        <v>259807.4346798256</v>
+      </c>
+      <c r="F707" t="n">
+        <v>259807.4346798256</v>
+      </c>
+      <c r="G707" t="n">
+        <v>270477.0726149913</v>
+      </c>
+      <c r="H707" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I707" t="inlineStr">
+        <is>
+          <t>KitKat</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" s="1" t="n">
+        <v>706</v>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>region: France24 brand: KitKat budget: 1200000</t>
+        </is>
+      </c>
+      <c r="C708" t="n">
+        <v>1200000.000000004</v>
+      </c>
+      <c r="D708" t="n">
+        <v>0</v>
+      </c>
+      <c r="E708" t="n">
+        <v>275692.7903816495</v>
+      </c>
+      <c r="F708" t="n">
+        <v>275692.7903816495</v>
+      </c>
+      <c r="G708" t="n">
+        <v>271178.7750243609</v>
+      </c>
+      <c r="H708" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I708" t="inlineStr">
+        <is>
+          <t>KitKat</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" s="1" t="n">
+        <v>707</v>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>region: France24 brand: KitKat budget: 1300000</t>
+        </is>
+      </c>
+      <c r="C709" t="n">
+        <v>1300000.00000335</v>
+      </c>
+      <c r="D709" t="n">
+        <v>0</v>
+      </c>
+      <c r="E709" t="n">
+        <v>290985.7594631944</v>
+      </c>
+      <c r="F709" t="n">
+        <v>290985.7594631944</v>
+      </c>
+      <c r="G709" t="n">
+        <v>271626.3703687684</v>
+      </c>
+      <c r="H709" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I709" t="inlineStr">
+        <is>
+          <t>KitKat</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" s="1" t="n">
+        <v>708</v>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>region: France24 brand: KitKat budget: 1400000</t>
+        </is>
+      </c>
+      <c r="C710" t="n">
+        <v>1400000.000000001</v>
+      </c>
+      <c r="D710" t="n">
+        <v>0</v>
+      </c>
+      <c r="E710" t="n">
+        <v>305731.066042278</v>
+      </c>
+      <c r="F710" t="n">
+        <v>305731.066042278</v>
+      </c>
+      <c r="G710" t="n">
+        <v>271911.8782844192</v>
+      </c>
+      <c r="H710" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I710" t="inlineStr">
+        <is>
+          <t>KitKat</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" s="1" t="n">
+        <v>709</v>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>region: France24 brand: KitKat budget: 1500000</t>
+        </is>
+      </c>
+      <c r="C711" t="n">
+        <v>1500000.000004334</v>
+      </c>
+      <c r="D711" t="n">
+        <v>0</v>
+      </c>
+      <c r="E711" t="n">
+        <v>319968.8288811258</v>
+      </c>
+      <c r="F711" t="n">
+        <v>319968.8288811258</v>
+      </c>
+      <c r="G711" t="n">
+        <v>272093.9953929404</v>
+      </c>
+      <c r="H711" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I711" t="inlineStr">
+        <is>
+          <t>KitKat</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" s="1" t="n">
+        <v>710</v>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>region: France24 brand: KitKat budget: 1600000</t>
+        </is>
+      </c>
+      <c r="C712" t="n">
+        <v>1600000.000000215</v>
+      </c>
+      <c r="D712" t="n">
+        <v>0</v>
+      </c>
+      <c r="E712" t="n">
+        <v>333721.2123987545</v>
+      </c>
+      <c r="F712" t="n">
+        <v>333721.2123987545</v>
+      </c>
+      <c r="G712" t="n">
+        <v>272210.1625441561</v>
+      </c>
+      <c r="H712" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I712" t="inlineStr">
+        <is>
+          <t>KitKat</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" s="1" t="n">
+        <v>711</v>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>region: France24 brand: KitKat budget: 1700000</t>
+        </is>
+      </c>
+      <c r="C713" t="n">
+        <v>1699999.99999995</v>
+      </c>
+      <c r="D713" t="n">
+        <v>0</v>
+      </c>
+      <c r="E713" t="n">
+        <v>343420.6638361102</v>
+      </c>
+      <c r="F713" t="n">
+        <v>343420.6638361102</v>
+      </c>
+      <c r="G713" t="n">
+        <v>272284.2621558456</v>
+      </c>
+      <c r="H713" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I713" t="inlineStr">
+        <is>
+          <t>KitKat</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" s="1" t="n">
+        <v>712</v>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>region: France24 brand: KitKat budget: 1800000</t>
+        </is>
+      </c>
+      <c r="C714" t="n">
+        <v>1799999.999998825</v>
+      </c>
+      <c r="D714" t="n">
+        <v>0</v>
+      </c>
+      <c r="E714" t="n">
+        <v>343925.3723188255</v>
+      </c>
+      <c r="F714" t="n">
+        <v>343925.3723188255</v>
+      </c>
+      <c r="G714" t="n">
+        <v>272331.528120404</v>
+      </c>
+      <c r="H714" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I714" t="inlineStr">
+        <is>
+          <t>KitKat</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" s="1" t="n">
+        <v>713</v>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>region: France24 brand: KitKat budget: 1900000</t>
+        </is>
+      </c>
+      <c r="C715" t="n">
+        <v>1899999.99999935</v>
+      </c>
+      <c r="D715" t="n">
+        <v>0</v>
+      </c>
+      <c r="E715" t="n">
+        <v>343925.3723192101</v>
+      </c>
+      <c r="F715" t="n">
+        <v>343925.3723192101</v>
+      </c>
+      <c r="G715" t="n">
+        <v>272361.6776900814</v>
+      </c>
+      <c r="H715" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I715" t="inlineStr">
+        <is>
+          <t>KitKat</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" s="1" t="n">
+        <v>714</v>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>region: France24 brand: KitKat budget: 200000</t>
+        </is>
+      </c>
+      <c r="C716" t="n">
+        <v>199999.9999999999</v>
+      </c>
+      <c r="D716" t="n">
+        <v>0</v>
+      </c>
+      <c r="E716" t="n">
+        <v>79617.35590666349</v>
+      </c>
+      <c r="F716" t="n">
+        <v>79617.35590666349</v>
+      </c>
+      <c r="G716" t="n">
+        <v>161574.9522721139</v>
+      </c>
+      <c r="H716" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I716" t="inlineStr">
+        <is>
+          <t>KitKat</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" s="1" t="n">
+        <v>715</v>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>region: France24 brand: KitKat budget: 2000000</t>
+        </is>
+      </c>
+      <c r="C717" t="n">
+        <v>1999999.999988884</v>
+      </c>
+      <c r="D717" t="n">
+        <v>0</v>
+      </c>
+      <c r="E717" t="n">
+        <v>343925.3723192101</v>
+      </c>
+      <c r="F717" t="n">
+        <v>343925.3723192101</v>
+      </c>
+      <c r="G717" t="n">
+        <v>272380.9092145012</v>
+      </c>
+      <c r="H717" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I717" t="inlineStr">
+        <is>
+          <t>KitKat</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" s="1" t="n">
+        <v>716</v>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>region: France24 brand: KitKat budget: 2100000</t>
+        </is>
+      </c>
+      <c r="C718" t="n">
+        <v>2099999.999999118</v>
+      </c>
+      <c r="D718" t="n">
+        <v>0</v>
+      </c>
+      <c r="E718" t="n">
+        <v>343925.3723192101</v>
+      </c>
+      <c r="F718" t="n">
+        <v>343925.3723192101</v>
+      </c>
+      <c r="G718" t="n">
+        <v>272393.1764387296</v>
+      </c>
+      <c r="H718" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I718" t="inlineStr">
+        <is>
+          <t>KitKat</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" s="1" t="n">
+        <v>717</v>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>region: France24 brand: KitKat budget: 300000</t>
+        </is>
+      </c>
+      <c r="C719" t="n">
+        <v>299999.9999999999</v>
+      </c>
+      <c r="D719" t="n">
+        <v>0</v>
+      </c>
+      <c r="E719" t="n">
+        <v>103968.1684381388</v>
+      </c>
+      <c r="F719" t="n">
+        <v>103968.1684381388</v>
+      </c>
+      <c r="G719" t="n">
+        <v>201713.3130180218</v>
+      </c>
+      <c r="H719" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I719" t="inlineStr">
+        <is>
+          <t>KitKat</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" s="1" t="n">
+        <v>718</v>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>region: France24 brand: KitKat budget: 400000</t>
+        </is>
+      </c>
+      <c r="C720" t="n">
+        <v>399999.9999999999</v>
+      </c>
+      <c r="D720" t="n">
+        <v>0</v>
+      </c>
+      <c r="E720" t="n">
+        <v>126989.3777049529</v>
+      </c>
+      <c r="F720" t="n">
+        <v>126989.3777049529</v>
+      </c>
+      <c r="G720" t="n">
+        <v>227316.393698304</v>
+      </c>
+      <c r="H720" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I720" t="inlineStr">
+        <is>
+          <t>KitKat</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" s="1" t="n">
+        <v>719</v>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>region: France24 brand: KitKat budget: 500000</t>
+        </is>
+      </c>
+      <c r="C721" t="n">
+        <v>500000.0000015063</v>
+      </c>
+      <c r="D721" t="n">
+        <v>0</v>
+      </c>
+      <c r="E721" t="n">
+        <v>148805.2832565431</v>
+      </c>
+      <c r="F721" t="n">
+        <v>148805.2832565431</v>
+      </c>
+      <c r="G721" t="n">
+        <v>243647.8464070621</v>
+      </c>
+      <c r="H721" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I721" t="inlineStr">
+        <is>
+          <t>KitKat</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" s="1" t="n">
+        <v>720</v>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>region: France24 brand: KitKat budget: 600000</t>
+        </is>
+      </c>
+      <c r="C722" t="n">
+        <v>600000.0000007135</v>
+      </c>
+      <c r="D722" t="n">
+        <v>0</v>
+      </c>
+      <c r="E722" t="n">
+        <v>169526.4780091974</v>
+      </c>
+      <c r="F722" t="n">
+        <v>169526.4780091974</v>
+      </c>
+      <c r="G722" t="n">
+        <v>254065.2001192645</v>
+      </c>
+      <c r="H722" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I722" t="inlineStr">
+        <is>
+          <t>KitKat</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" s="1" t="n">
+        <v>721</v>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>region: France24 brand: KitKat budget: 700000</t>
+        </is>
+      </c>
+      <c r="C723" t="n">
+        <v>699999.9999999995</v>
+      </c>
+      <c r="D723" t="n">
+        <v>0</v>
+      </c>
+      <c r="E723" t="n">
+        <v>189251.3260789057</v>
+      </c>
+      <c r="F723" t="n">
+        <v>189251.3260789057</v>
+      </c>
+      <c r="G723" t="n">
+        <v>260710.1238932595</v>
+      </c>
+      <c r="H723" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I723" t="inlineStr">
+        <is>
+          <t>KitKat</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" s="1" t="n">
+        <v>722</v>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>region: France24 brand: KitKat budget: 800000</t>
+        </is>
+      </c>
+      <c r="C724" t="n">
+        <v>799999.9999999859</v>
+      </c>
+      <c r="D724" t="n">
+        <v>0</v>
+      </c>
+      <c r="E724" t="n">
+        <v>208067.8732257186</v>
+      </c>
+      <c r="F724" t="n">
+        <v>208067.8732257186</v>
+      </c>
+      <c r="G724" t="n">
+        <v>264948.72547887</v>
+      </c>
+      <c r="H724" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I724" t="inlineStr">
+        <is>
+          <t>KitKat</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" s="1" t="n">
+        <v>723</v>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>region: France24 brand: KitKat budget: 900000</t>
+        </is>
+      </c>
+      <c r="C725" t="n">
+        <v>900000.0000000003</v>
+      </c>
+      <c r="D725" t="n">
+        <v>0</v>
+      </c>
+      <c r="E725" t="n">
+        <v>226054.0474294396</v>
+      </c>
+      <c r="F725" t="n">
+        <v>226054.0474294396</v>
+      </c>
+      <c r="G725" t="n">
+        <v>267652.4048606707</v>
+      </c>
+      <c r="H725" t="inlineStr">
+        <is>
+          <t>France24</t>
+        </is>
+      </c>
+      <c r="I725" t="inlineStr">
+        <is>
+          <t>KitKat</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>